<commit_message>
added new data and streamlit app haven't updated in a while
</commit_message>
<xml_diff>
--- a/Lombardia_processed/PO013035NU0002_2014_2021.xlsx
+++ b/Lombardia_processed/PO013035NU0002_2014_2021.xlsx
@@ -1,60 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="4">
-  <si>
-    <t>CODICE PUNTO</t>
-  </si>
-  <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>MISURA SOGGIACENZA [m]</t>
-  </si>
-  <si>
-    <t>PO013035NU0002</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -69,36 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -386,377 +424,549 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>codice</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>val</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>41729</v>
+      </c>
+      <c r="D2" t="n">
+        <v>13.68</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>41822</v>
+      </c>
+      <c r="D3" t="n">
+        <v>13.46</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>41912</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10.72</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>41729</v>
-      </c>
-      <c r="C2">
-        <v>13.68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>41822</v>
-      </c>
-      <c r="C3">
-        <v>13.46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>41912</v>
-      </c>
-      <c r="C4">
-        <v>10.72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>41913</v>
       </c>
-      <c r="C5">
+      <c r="D5" t="n">
         <v>12.17</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>41960</v>
       </c>
-      <c r="C6">
+      <c r="D6" t="n">
         <v>10.45</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2">
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
         <v>42130</v>
       </c>
-      <c r="C7">
+      <c r="D7" t="n">
         <v>9.609999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2">
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>42296</v>
       </c>
-      <c r="C8">
+      <c r="D8" t="n">
         <v>14.46</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>42422</v>
       </c>
-      <c r="C9">
+      <c r="D9" t="n">
         <v>16.47</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2">
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>42480</v>
       </c>
-      <c r="C10">
+      <c r="D10" t="n">
         <v>18.32</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
         <v>42557</v>
       </c>
-      <c r="C11">
+      <c r="D11" t="n">
         <v>19.91</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>42676</v>
       </c>
-      <c r="C12">
+      <c r="D12" t="n">
         <v>18.42</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2">
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
         <v>42783</v>
       </c>
-      <c r="C13">
+      <c r="D13" t="n">
         <v>19.04</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="2">
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
         <v>42865</v>
       </c>
-      <c r="C14">
+      <c r="D14" t="n">
         <v>19.51</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2">
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
         <v>42936</v>
       </c>
-      <c r="C15">
+      <c r="D15" t="n">
         <v>20.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2">
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
         <v>43027</v>
       </c>
-      <c r="C16">
+      <c r="D16" t="n">
         <v>20.3</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="2">
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
         <v>43143</v>
       </c>
-      <c r="C17">
+      <c r="D17" t="n">
         <v>20.8</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="2">
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
         <v>43214</v>
       </c>
-      <c r="C18">
+      <c r="D18" t="n">
         <v>20.7</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="2">
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
         <v>43287</v>
       </c>
-      <c r="C19">
+      <c r="D19" t="n">
         <v>20.4</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2">
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
         <v>43413</v>
       </c>
-      <c r="C20">
+      <c r="D20" t="n">
         <v>20.36</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="2">
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
         <v>43518</v>
       </c>
-      <c r="C21">
+      <c r="D21" t="n">
         <v>20.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="2">
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
         <v>43598</v>
       </c>
-      <c r="C22">
+      <c r="D22" t="n">
         <v>21.12</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="2">
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
         <v>43661</v>
       </c>
-      <c r="C23">
+      <c r="D23" t="n">
         <v>22.2</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="2">
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
         <v>43762</v>
       </c>
-      <c r="C24">
+      <c r="D24" t="n">
         <v>22.3</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="2">
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
         <v>43878</v>
       </c>
-      <c r="C25">
+      <c r="D25" t="n">
         <v>19.12</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="2">
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
         <v>43910</v>
       </c>
-      <c r="C26">
+      <c r="D26" t="n">
         <v>20.42</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="2">
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
         <v>44002</v>
       </c>
-      <c r="C27">
+      <c r="D27" t="n">
         <v>19.97</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="2">
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
         <v>44094</v>
       </c>
-      <c r="C28">
+      <c r="D28" t="n">
         <v>18.42</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="2">
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
         <v>44116</v>
       </c>
-      <c r="C29">
+      <c r="D29" t="n">
         <v>23.3</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="2">
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
         <v>44185</v>
       </c>
-      <c r="C30">
+      <c r="D30" t="n">
         <v>18.27</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="2">
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
         <v>44307</v>
       </c>
-      <c r="C31">
+      <c r="D31" t="n">
         <v>18.3</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="2">
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
         <v>44348</v>
       </c>
-      <c r="C32">
+      <c r="D32" t="n">
         <v>18.65</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="2">
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>PO013035NU0002</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
         <v>44440</v>
       </c>
-      <c r="C33">
+      <c r="D33" t="n">
         <v>19.1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>